<commit_message>
Veri setinin uygulamadan okunması ve veri setinin genişletilmesi - İP (İş Paketi) No: 5
Veri setine aynı bölgeden olmak üzere 20 tane daha veri eklendi. Veri seti girişler ve çıkışlar olmak üzere sütunlarına göre ayrıldı. Transpoz işlemi yapılarak değişkenlere atandı.  Oluşturulan değişkenler global hale getirildi ve workspace içine kaydedildi.
</commit_message>
<xml_diff>
--- a/veriSeti.xlsx
+++ b/veriSeti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erkan\Documents\GitHub\ev-fiyat-tahmini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009ADDC1-1330-49AF-9463-C818556364FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660D8986-4FA2-430D-BE11-5B139F6212AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="645" windowWidth="22905" windowHeight="13560" xr2:uid="{BA7FDC94-C96F-4FB8-B0A9-928190BC2284}"/>
+    <workbookView xWindow="4470" yWindow="2130" windowWidth="22905" windowHeight="13560" xr2:uid="{BA7FDC94-C96F-4FB8-B0A9-928190BC2284}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -494,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C7BBD2-ED17-4E1C-8752-C66538F24EF9}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,6 +1812,646 @@
         <v>185000</v>
       </c>
     </row>
+    <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>160</v>
+      </c>
+      <c r="B42" s="3">
+        <v>150</v>
+      </c>
+      <c r="C42" s="3">
+        <v>3</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
+        <v>13</v>
+      </c>
+      <c r="F42" s="3">
+        <v>3</v>
+      </c>
+      <c r="G42" s="3">
+        <v>44</v>
+      </c>
+      <c r="H42" s="3">
+        <v>1</v>
+      </c>
+      <c r="I42" s="3">
+        <v>0</v>
+      </c>
+      <c r="J42" s="4">
+        <v>325000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>170</v>
+      </c>
+      <c r="B43" s="3">
+        <v>140</v>
+      </c>
+      <c r="C43" s="3">
+        <v>3</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <v>18</v>
+      </c>
+      <c r="F43" s="3">
+        <v>4</v>
+      </c>
+      <c r="G43" s="3">
+        <v>4</v>
+      </c>
+      <c r="H43" s="3">
+        <v>1</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1</v>
+      </c>
+      <c r="J43" s="4">
+        <v>277000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>350</v>
+      </c>
+      <c r="B44" s="3">
+        <v>260</v>
+      </c>
+      <c r="C44" s="3">
+        <v>5</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3">
+        <v>18</v>
+      </c>
+      <c r="F44" s="3">
+        <v>3</v>
+      </c>
+      <c r="G44" s="3">
+        <v>4</v>
+      </c>
+      <c r="H44" s="3">
+        <v>1</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0</v>
+      </c>
+      <c r="J44" s="4">
+        <v>410000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>135</v>
+      </c>
+      <c r="B45" s="3">
+        <v>105</v>
+      </c>
+      <c r="C45" s="3">
+        <v>2</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1</v>
+      </c>
+      <c r="E45" s="3">
+        <v>28</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3">
+        <v>3</v>
+      </c>
+      <c r="H45" s="3">
+        <v>1</v>
+      </c>
+      <c r="I45" s="3">
+        <v>0</v>
+      </c>
+      <c r="J45" s="4">
+        <v>227000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>145</v>
+      </c>
+      <c r="B46" s="3">
+        <v>125</v>
+      </c>
+      <c r="C46" s="3">
+        <v>3</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
+        <v>2</v>
+      </c>
+      <c r="G46" s="3">
+        <v>4</v>
+      </c>
+      <c r="H46" s="3">
+        <v>1</v>
+      </c>
+      <c r="I46" s="3">
+        <v>0</v>
+      </c>
+      <c r="J46" s="4">
+        <v>314000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>180</v>
+      </c>
+      <c r="B47" s="3">
+        <v>150</v>
+      </c>
+      <c r="C47" s="3">
+        <v>3</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1</v>
+      </c>
+      <c r="E47" s="3">
+        <v>28</v>
+      </c>
+      <c r="F47" s="3">
+        <v>5</v>
+      </c>
+      <c r="G47" s="3">
+        <v>5</v>
+      </c>
+      <c r="H47" s="3">
+        <v>2</v>
+      </c>
+      <c r="I47" s="3">
+        <v>0</v>
+      </c>
+      <c r="J47" s="4">
+        <v>325000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>160</v>
+      </c>
+      <c r="B48" s="3">
+        <v>140</v>
+      </c>
+      <c r="C48" s="3">
+        <v>3</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
+        <v>28</v>
+      </c>
+      <c r="F48" s="3">
+        <v>5</v>
+      </c>
+      <c r="G48" s="3">
+        <v>5</v>
+      </c>
+      <c r="H48" s="3">
+        <v>1</v>
+      </c>
+      <c r="I48" s="3">
+        <v>0</v>
+      </c>
+      <c r="J48" s="4">
+        <v>260000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>115</v>
+      </c>
+      <c r="B49" s="3">
+        <v>95</v>
+      </c>
+      <c r="C49" s="3">
+        <v>2</v>
+      </c>
+      <c r="D49" s="3">
+        <v>1</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>2</v>
+      </c>
+      <c r="G49" s="3">
+        <v>4</v>
+      </c>
+      <c r="H49" s="3">
+        <v>1</v>
+      </c>
+      <c r="I49" s="3">
+        <v>0</v>
+      </c>
+      <c r="J49" s="4">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>110</v>
+      </c>
+      <c r="B50" s="3">
+        <v>100</v>
+      </c>
+      <c r="C50" s="3">
+        <v>2</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
+        <v>2</v>
+      </c>
+      <c r="G50" s="3">
+        <v>3</v>
+      </c>
+      <c r="H50" s="3">
+        <v>1</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0</v>
+      </c>
+      <c r="J50" s="4">
+        <v>310000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>400</v>
+      </c>
+      <c r="B51" s="3">
+        <v>350</v>
+      </c>
+      <c r="C51" s="3">
+        <v>6</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3">
+        <v>13</v>
+      </c>
+      <c r="F51" s="3">
+        <v>4</v>
+      </c>
+      <c r="G51" s="3">
+        <v>5</v>
+      </c>
+      <c r="H51" s="3">
+        <v>1</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
+      <c r="J51" s="4">
+        <v>435000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>120</v>
+      </c>
+      <c r="B52" s="3">
+        <v>95</v>
+      </c>
+      <c r="C52" s="3">
+        <v>2</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3">
+        <v>4</v>
+      </c>
+      <c r="H52" s="3">
+        <v>1</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0</v>
+      </c>
+      <c r="J52" s="4">
+        <v>199000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>150</v>
+      </c>
+      <c r="B53" s="3">
+        <v>130</v>
+      </c>
+      <c r="C53" s="3">
+        <v>3</v>
+      </c>
+      <c r="D53" s="3">
+        <v>1</v>
+      </c>
+      <c r="E53" s="3">
+        <v>28</v>
+      </c>
+      <c r="F53" s="3">
+        <v>3</v>
+      </c>
+      <c r="G53" s="3">
+        <v>5</v>
+      </c>
+      <c r="H53" s="3">
+        <v>1</v>
+      </c>
+      <c r="I53" s="3">
+        <v>0</v>
+      </c>
+      <c r="J53" s="4">
+        <v>235000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>120</v>
+      </c>
+      <c r="B54" s="3">
+        <v>100</v>
+      </c>
+      <c r="C54" s="3">
+        <v>2</v>
+      </c>
+      <c r="D54" s="3">
+        <v>1</v>
+      </c>
+      <c r="E54" s="3">
+        <v>35</v>
+      </c>
+      <c r="F54" s="3">
+        <v>5</v>
+      </c>
+      <c r="G54" s="3">
+        <v>6</v>
+      </c>
+      <c r="H54" s="3">
+        <v>1</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0</v>
+      </c>
+      <c r="J54" s="4">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>170</v>
+      </c>
+      <c r="B55" s="3">
+        <v>145</v>
+      </c>
+      <c r="C55" s="3">
+        <v>3</v>
+      </c>
+      <c r="D55" s="3">
+        <v>1</v>
+      </c>
+      <c r="E55" s="3">
+        <v>13</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3">
+        <v>5</v>
+      </c>
+      <c r="H55" s="3">
+        <v>1</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0</v>
+      </c>
+      <c r="J55" s="4">
+        <v>327000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>160</v>
+      </c>
+      <c r="B56" s="3">
+        <v>145</v>
+      </c>
+      <c r="C56" s="3">
+        <v>3</v>
+      </c>
+      <c r="D56" s="3">
+        <v>1</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3">
+        <v>2</v>
+      </c>
+      <c r="G56" s="3">
+        <v>4</v>
+      </c>
+      <c r="H56" s="3">
+        <v>1</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0</v>
+      </c>
+      <c r="J56" s="4">
+        <v>480000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>147</v>
+      </c>
+      <c r="B57" s="3">
+        <v>137</v>
+      </c>
+      <c r="C57" s="3">
+        <v>3</v>
+      </c>
+      <c r="D57" s="3">
+        <v>1</v>
+      </c>
+      <c r="E57" s="3">
+        <v>8</v>
+      </c>
+      <c r="F57" s="3">
+        <v>0</v>
+      </c>
+      <c r="G57" s="3">
+        <v>13</v>
+      </c>
+      <c r="H57" s="3">
+        <v>1</v>
+      </c>
+      <c r="I57" s="3">
+        <v>1</v>
+      </c>
+      <c r="J57" s="4">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>164</v>
+      </c>
+      <c r="B58" s="3">
+        <v>140</v>
+      </c>
+      <c r="C58" s="3">
+        <v>3</v>
+      </c>
+      <c r="D58" s="3">
+        <v>1</v>
+      </c>
+      <c r="E58" s="3">
+        <v>28</v>
+      </c>
+      <c r="F58" s="3">
+        <v>2</v>
+      </c>
+      <c r="G58" s="3">
+        <v>5</v>
+      </c>
+      <c r="H58" s="3">
+        <v>3</v>
+      </c>
+      <c r="I58" s="3">
+        <v>0</v>
+      </c>
+      <c r="J58" s="4">
+        <v>169900</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>115</v>
+      </c>
+      <c r="B59" s="3">
+        <v>100</v>
+      </c>
+      <c r="C59" s="3">
+        <v>2</v>
+      </c>
+      <c r="D59" s="3">
+        <v>1</v>
+      </c>
+      <c r="E59" s="3">
+        <v>23</v>
+      </c>
+      <c r="F59" s="3">
+        <v>1</v>
+      </c>
+      <c r="G59" s="3">
+        <v>4</v>
+      </c>
+      <c r="H59" s="3">
+        <v>3</v>
+      </c>
+      <c r="I59" s="3">
+        <v>0</v>
+      </c>
+      <c r="J59" s="4">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>150</v>
+      </c>
+      <c r="B60" s="3">
+        <v>125</v>
+      </c>
+      <c r="C60" s="3">
+        <v>3</v>
+      </c>
+      <c r="D60" s="3">
+        <v>1</v>
+      </c>
+      <c r="E60" s="3">
+        <v>35</v>
+      </c>
+      <c r="F60" s="3">
+        <v>4</v>
+      </c>
+      <c r="G60" s="3">
+        <v>5</v>
+      </c>
+      <c r="H60" s="3">
+        <v>3</v>
+      </c>
+      <c r="I60" s="3">
+        <v>0</v>
+      </c>
+      <c r="J60" s="4">
+        <v>137000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>120</v>
+      </c>
+      <c r="B61" s="3">
+        <v>112</v>
+      </c>
+      <c r="C61" s="3">
+        <v>2</v>
+      </c>
+      <c r="D61" s="3">
+        <v>1</v>
+      </c>
+      <c r="E61" s="3">
+        <v>28</v>
+      </c>
+      <c r="F61" s="3">
+        <v>4</v>
+      </c>
+      <c r="G61" s="3">
+        <v>6</v>
+      </c>
+      <c r="H61" s="3">
+        <v>3</v>
+      </c>
+      <c r="I61" s="3">
+        <v>0</v>
+      </c>
+      <c r="J61" s="4">
+        <v>138000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>